<commit_message>
iRecorderQuestion 测试通过 iRecorderScore 测试通过 待整合与完善
</commit_message>
<xml_diff>
--- a/doc/座席录音质检资源接口说明文档.xlsx
+++ b/doc/座席录音质检资源接口说明文档.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>
     <sheet name="Post" sheetId="5" r:id="rId2"/>
+    <sheet name="Put" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="60">
   <si>
     <t>REST接口说明</t>
   </si>
@@ -199,6 +200,46 @@
   </si>
   <si>
     <t>Json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/irecorderservice/irecorderscore?filename=10.4.48.29_20130401090313511_5_3186_37043.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试Json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"total": "3.08", "scrvals": "C001#2|C002#2|C003#0|C004#2|C006#2|C005#3|C007#1|C008#1|C009#1|C010#1|C011#2|C012#1|C013#9|C014#6|C015#6|", "fileName": "10.4.48.29_20130401090313511_5_3186_37043.wav","remark": "test only", "raters": "37014", "reterTime": "2013-04-15 15:04:48"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'total': Decimal('5.08'), 'scrvals': 'C001#2|C002#2|C003#0|C004#2|C006#2|C005#3|C007#1|C008#1|C009#1|C010#1|C011#2|C012#1|C013#9|C014#6|C015#6|', 'scrval14': '', 'scrval15': '', 'scrval12': '', 'scrval13': '', 'scrval10': '', 'scrval11': '', 'fileName': '10.4.48.29_20121024145206943_3_3184_37001.wav', 'scrval8': '', 'scrval9': '', 'scrval4': '', 'scrval5': '', 'scrval6': '', 'scrval7': '', 'scrval0': '', 'scrval1': '', 'scrval2': '', 'scrval3': '', 'remark': 'test only', 'raters': '37014', 'reterTime': '2013-05-28 15:19:17'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'total': Decimal('3.08'), 'scrvals': 'C001#2|C002#2|C003#0|C004#2|C006#2|C005#3|C007#1|C008#1|C009#1|C010#1|C011#2|C012#1|C013#9|C014#6|C015#6|', 'scrval14': None, 'scrval15': None, 'scrval12': None, 'scrval13': None, 'scrval10': None, 'scrval11': None, 'fileName': '10.4.48.29_20130401090313511_5_3186_37043.wav', 'scrval8': None, 'scrval9': None, 'scrval4': None, 'scrval5': None, 'scrval6': None, 'scrval7': None, 'scrval0': None, 'scrval1': None, 'scrval2': None, 'scrval3': None, 'remark': '\xbb\xa5\xb6\xaf\xc9\xd9\xa3\xac\xcc\xbd\xd1\xaf\xb2\xbb\xb9\xbb\xa3\xac\xcc\xd8\xb1\xf0\xca\xc7\xb6\xd4\xbe\xba\xc6\xb7\xb5\xc4\xb9\xfd\xb6\xc9\xb2\xbb\xb9\xbb\r\n\xc1\xed\xa3\xba\xce\xb4\xb0\xb4\xbf\xda\xca\xf6\xb8\xe5\xd3\xaa\xd1\xf8\xbd\xa8\xd2\xe9\xc1\xf7\xb3\xcc\xa3\xac\xce\xb4\xcc\xe1\xbc\xb0\xd4\xa4\xb2\xfa\xc6\xda\xc8\xb7\xc8\xcf', 'raters': '37014', 'reterTime': '2013-04-15 15:04:48'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Put</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增一条录音质检的信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改一条录音质检的信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"total": "7.6", "scrvals": "C001#2|C002#2|C003#0|C004#2|C006#2|C005#3|C007#1|C008#1|C009#1|C010#1|C011#2|C012#1|C013#9|C014#6|C015#6|", "fileName": "10.4.48.29_20130401090313511_5_3186_37043.wav","remark": "test only", "raters": "37014", "reterTime": "2013-04-15 15:04:48"}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -344,7 +385,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -390,6 +431,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -398,6 +445,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -751,21 +807,21 @@
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
@@ -897,41 +953,55 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" s="14" customFormat="1">
       <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="12"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
     </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -941,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -987,7 +1057,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>2</v>
@@ -1000,21 +1070,21 @@
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
@@ -1146,41 +1216,318 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" s="14" customFormat="1">
       <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="12"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
     </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="30.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18" style="8" customWidth="1"/>
+    <col min="4" max="4" width="41.375" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="22.5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="18.75">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="40.5">
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="5"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>